<commit_message>
Make sure the excel importer works + editor separator color
</commit_message>
<xml_diff>
--- a/Assets/Excel/MasterItem.xlsx
+++ b/Assets/Excel/MasterItem.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\_VincentGame\HorrorGame\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FA2E06D-C977-4221-A1A4-F1B69CEBB592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C9F73BE-ED0A-45B2-B45F-A8648C5B1685}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{CE5CDD7E-8CFD-476C-AB84-63CE99224655}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ItemList" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -421,7 +421,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J20" sqref="J20"/>
+      <selection activeCell="I21" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>